<commit_message>
Export test file improved with sample transactions
</commit_message>
<xml_diff>
--- a/tests/export_waltio_test.xlsx
+++ b/tests/export_waltio_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\Dev\Crypto\waltio\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Documents\Dev\Crypto\waltio\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB41209D-0BC4-4EFA-9F1C-A629F5D8E877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550530D1-D851-446F-9D43-2E75E5D87BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="38700" windowHeight="11460" xr2:uid="{E9DE087D-10DA-DD4C-9ED2-E4FA50E230DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9DE087D-10DA-DD4C-9ED2-E4FA50E230DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Vos données" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="128">
   <si>
     <t>Type</t>
   </si>
@@ -315,6 +315,105 @@
   </si>
   <si>
     <t>ext-id-3</t>
+  </si>
+  <si>
+    <t>SOL</t>
+  </si>
+  <si>
+    <t>Kraken</t>
+  </si>
+  <si>
+    <t>Achat de SOL via Moonpay</t>
+  </si>
+  <si>
+    <t>tx-hash-1</t>
+  </si>
+  <si>
+    <t>ext-id-4</t>
+  </si>
+  <si>
+    <t>EGLD</t>
+  </si>
+  <si>
+    <t>kraken</t>
+  </si>
+  <si>
+    <t>Swap SOL vers EGLD</t>
+  </si>
+  <si>
+    <t>ext-id-5</t>
+  </si>
+  <si>
+    <t>adr-1</t>
+  </si>
+  <si>
+    <t>Achat DCA EGLD</t>
+  </si>
+  <si>
+    <t>ext-id-6</t>
+  </si>
+  <si>
+    <t>Vente Ethereum</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>ext-id-7</t>
+  </si>
+  <si>
+    <t>Retrait sur Ledger</t>
+  </si>
+  <si>
+    <t>adr-2</t>
+  </si>
+  <si>
+    <t>tx-hash-2</t>
+  </si>
+  <si>
+    <t>ext-id-8</t>
+  </si>
+  <si>
+    <t>Ledger wallet</t>
+  </si>
+  <si>
+    <t>01/06/2021 07:18:18</t>
+  </si>
+  <si>
+    <t>01/06/2021 07:20:18</t>
+  </si>
+  <si>
+    <t>04/06/2021 10:28:12</t>
+  </si>
+  <si>
+    <t>13/06/2021 16:38:42</t>
+  </si>
+  <si>
+    <t>20/06/2021 16:24:06</t>
+  </si>
+  <si>
+    <t>27/06/2021 10:04:42</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Vente de SOL</t>
+  </si>
+  <si>
+    <t>ext-id-9</t>
+  </si>
+  <si>
+    <t>03/10/2021 21:33:12</t>
+  </si>
+  <si>
+    <t>Vente de USDT</t>
+  </si>
+  <si>
+    <t>ext-id-10</t>
+  </si>
+  <si>
+    <t>12/10/2021 13:37:48</t>
   </si>
 </sst>
 </file>
@@ -396,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,11 +523,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -777,40 +906,40 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="96.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="62.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="92" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="174.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.8984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.09765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.69921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -862,11 +991,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -896,11 +1025,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -948,11 +1077,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1000,25 +1129,406 @@
         <v>94</v>
       </c>
     </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="6">
+        <v>140</v>
+      </c>
+      <c r="P5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="6">
+        <v>135</v>
+      </c>
+      <c r="N6" s="6">
+        <v>21.6</v>
+      </c>
+      <c r="O6" s="6">
+        <v>135</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="6">
+        <v>50</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>25</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="6">
+        <v>5000</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1.002</v>
+      </c>
+      <c r="O8" s="6">
+        <v>5000</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6">
+        <v>500</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="P9" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>112</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6">
+        <v>500</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="P10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" s="12"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3450</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6">
+        <v>690</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O11" s="6">
+        <v>690</v>
+      </c>
+      <c r="R11" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6">
+        <v>250</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="6">
+        <v>250</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
       <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B10">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>AND(LEN(#REF!)&gt;0,LEN(#REF!)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1028,7 +1538,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{D7B294F2-3B9E-4B10-8E14-2837B346429E}">
+          <x14:cfRule type="expression" priority="8" id="{D7B294F2-3B9E-4B10-8E14-2837B346429E}">
             <xm:f>AND(COUNTIF(Dictionnaire!$A$2:$A$4,A3)=0,LEN(A3)&gt;0)</xm:f>
             <x14:dxf>
               <fill>
@@ -1040,6 +1550,19 @@
           </x14:cfRule>
           <xm:sqref>A3:A4</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{B45D6741-90BB-444F-BEDF-638B5B914A1C}">
+            <xm:f>AND(COUNTIF(Dictionnaire!$A$2:$A$4,A6)=0,LEN(A6)&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A6:A12</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1048,7 +1571,7 @@
           <x14:formula1>
             <xm:f>Dictionnaire!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A4</xm:sqref>
+          <xm:sqref>A3:A4 A6:A8 A11:A12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{14EAAC43-44BF-6E4F-8A93-B2A5D1C7E463}">
           <x14:formula1>
@@ -1079,20 +1602,20 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1635,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1644,7 @@
       </c>
       <c r="C2" s="3">
         <f ca="1">NOW()</f>
-        <v>45527.39667962963</v>
+        <v>45527.591048842594</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
@@ -1133,7 +1656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>64</v>
       </c>
@@ -1172,7 +1695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>57</v>
       </c>
@@ -1194,7 +1717,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>61</v>
       </c>
@@ -1205,7 +1728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -1216,7 +1739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>58</v>
       </c>
@@ -1227,7 +1750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1238,7 +1761,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>63</v>
       </c>
@@ -1249,7 +1772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>74</v>
       </c>
@@ -1260,7 +1783,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>75</v>
       </c>
@@ -1271,7 +1794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>76</v>
       </c>
@@ -1282,7 +1805,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>77</v>
       </c>
@@ -1293,7 +1816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>78</v>
       </c>
@@ -1301,7 +1824,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>80</v>
       </c>
@@ -1309,7 +1832,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>81</v>
       </c>
@@ -1317,7 +1840,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>72</v>
       </c>
@@ -1325,62 +1848,62 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>54</v>
       </c>

</xml_diff>